<commit_message>
updated BOM to match order
</commit_message>
<xml_diff>
--- a/Hardware/ALL-BOM.xlsx
+++ b/Hardware/ALL-BOM.xlsx
@@ -9,20 +9,25 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="753" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Power Outlet-BOM" sheetId="1" r:id="rId1"/>
-    <sheet name="Beaglebone Cape" sheetId="4" r:id="rId2"/>
-    <sheet name="Mouser Order" sheetId="3" r:id="rId3"/>
-    <sheet name="Heating Controller BOM" sheetId="2" r:id="rId4"/>
+    <sheet name="Beaglebone Cape Rev A." sheetId="4" r:id="rId2"/>
+    <sheet name="nrf24L01" sheetId="5" r:id="rId3"/>
+    <sheet name="PoE" sheetId="6" r:id="rId4"/>
+    <sheet name="Energry Sensor" sheetId="7" r:id="rId5"/>
+    <sheet name="Environment Sensor" sheetId="8" r:id="rId6"/>
+    <sheet name="Lighting Controller" sheetId="9" r:id="rId7"/>
+    <sheet name="Heating Controller BOM" sheetId="2" r:id="rId8"/>
+    <sheet name="Mouser Order" sheetId="3" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="174">
   <si>
     <t>Qty</t>
   </si>
@@ -466,13 +471,91 @@
   </si>
   <si>
     <t>42M2667</t>
+  </si>
+  <si>
+    <t>En</t>
+  </si>
+  <si>
+    <t>Power Outlet</t>
+  </si>
+  <si>
+    <t>nrf24l01(3)</t>
+  </si>
+  <si>
+    <t>71-CRCW1206-0-E3</t>
+  </si>
+  <si>
+    <t>0 Ohm 1206 resistor</t>
+  </si>
+  <si>
+    <t>EnergySensor</t>
+  </si>
+  <si>
+    <t>Mains MOV</t>
+  </si>
+  <si>
+    <t>Heating Controller</t>
+  </si>
+  <si>
+    <t>634-SI7006-A20-IM</t>
+  </si>
+  <si>
+    <t>Humidity &amp; Temp Sensor</t>
+  </si>
+  <si>
+    <t>Relay</t>
+  </si>
+  <si>
+    <t>Lightswitch</t>
+  </si>
+  <si>
+    <t>Env Sensor(2)</t>
+  </si>
+  <si>
+    <t>Ambient Light Sensor</t>
+  </si>
+  <si>
+    <t>630-APDS-9007-020</t>
+  </si>
+  <si>
+    <t>Atmega328p-AU</t>
+  </si>
+  <si>
+    <t>556-ATMEGA328P-AU</t>
+  </si>
+  <si>
+    <t>OptoIsolator</t>
+  </si>
+  <si>
+    <t>22p cap</t>
+  </si>
+  <si>
+    <t>80-C1206C130J5G</t>
+  </si>
+  <si>
+    <t>14 p cap</t>
+  </si>
+  <si>
+    <t>0.1u 275</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>10uH</t>
+  </si>
+  <si>
+    <t>0.1u cap</t>
+  </si>
+  <si>
+    <t>70-ILSB1206ER100K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,6 +689,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -960,7 +1049,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -970,6 +1059,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1312,8 +1402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,11 +1989,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -2133,103 +2226,51 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2237,7 +2278,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2249,4 +2302,336 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" t="s">
+        <v>150</v>
+      </c>
+      <c r="F1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I1" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>SUM(D2:J2)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f>SUM(D3:J3)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <f>SUM(D4:J4)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f>SUM(D5:J5)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <f>SUM(D6:J6)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f>SUM(D7:J7)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <f>SUM(D8:J8)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <f>SUM(D9:J9)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <f>SUM(D10:J10)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <f>SUM(D11:J11)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" t="s">
+        <v>151</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+      <c r="K12">
+        <f>SUM(D12:J12)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <f>SUM(D13:J13)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" t="s">
+        <v>162</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <f>SUM(D14:J14)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C15" t="s">
+        <v>164</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <f>SUM(D15:J15)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
+      <c r="K16">
+        <f>SUM(D16:J16)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C17" t="s">
+        <v>173</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added manufacturing pictures, tidied code and commented. prepared for final commit ready for submission
</commit_message>
<xml_diff>
--- a/Hardware/ALL-BOM.xlsx
+++ b/Hardware/ALL-BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="753" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" tabRatio="753" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Power Outlet-BOM" sheetId="1" r:id="rId1"/>
@@ -820,10 +820,10 @@
     <t>Item</t>
   </si>
   <si>
-    <t>Total Costs</t>
-  </si>
-  <si>
     <t>Total Available</t>
+  </si>
+  <si>
+    <t>Balance</t>
   </si>
 </sst>
 </file>
@@ -1382,42 +1382,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="34" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <font>
         <b val="0"/>
@@ -1507,6 +1472,58 @@
       </font>
       <numFmt numFmtId="34" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1532,7 +1549,7 @@
     <tableColumn id="6" name="Description"/>
     <tableColumn id="10" name="OrderNo (Rapid/Mouser)"/>
     <tableColumn id="7" name="Cost (Ea)" totalsRowLabel="Total"/>
-    <tableColumn id="8" name="Cost" totalsRowFunction="custom" totalsRowDxfId="6" dataCellStyle="Currency">
+    <tableColumn id="8" name="Cost" totalsRowFunction="custom" totalsRowDxfId="7" dataCellStyle="Currency">
       <calculatedColumnFormula>Table1[[#This Row],[Cost (Ea)]]*Table1[[#This Row],[Qty]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(I2:I22)</totalsRowFormula>
     </tableColumn>
@@ -1542,12 +1559,12 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A20:B24" totalsRowCount="1">
-  <autoFilter ref="A20:B24"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="G2:H6" totalsRowCount="1">
+  <autoFilter ref="G2:H5"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Item" totalsRowLabel="Total Available"/>
-    <tableColumn id="2" name="Cost" totalsRowFunction="custom" dataCellStyle="Currency">
-      <totalsRowFormula>SUM(B21:B23)</totalsRowFormula>
+    <tableColumn id="2" name="Cost" totalsRowFunction="custom" totalsRowDxfId="0" dataCellStyle="Currency">
+      <totalsRowFormula>SUM(H3:H5)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1566,7 +1583,7 @@
     <tableColumn id="6" name="Description"/>
     <tableColumn id="8" name="OrderNo (Rapid/Mouser)"/>
     <tableColumn id="9" name="Cost (Ea)" totalsRowLabel="Total"/>
-    <tableColumn id="10" name="Cost" totalsRowFunction="custom" totalsRowDxfId="1" dataCellStyle="Currency">
+    <tableColumn id="10" name="Cost" totalsRowFunction="custom" totalsRowDxfId="6" dataCellStyle="Currency">
       <calculatedColumnFormula>Table2[[#This Row],[Cost (Ea)]]*Table2[[#This Row],[Qty]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(I2:I4)</totalsRowFormula>
     </tableColumn>
@@ -1577,7 +1594,7 @@
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A1:I8" totalsRowCount="1">
-  <autoFilter ref="A1:I8"/>
+  <autoFilter ref="A1:I7"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Qty"/>
     <tableColumn id="2" name="Value"/>
@@ -1587,7 +1604,7 @@
     <tableColumn id="6" name="Description"/>
     <tableColumn id="8" name="OrderNo (Rapid/Mouser)"/>
     <tableColumn id="9" name="Cost (Ea)" totalsRowLabel="Total"/>
-    <tableColumn id="10" name="Cost" totalsRowFunction="custom" totalsRowDxfId="2" dataCellStyle="Currency">
+    <tableColumn id="10" name="Cost" totalsRowFunction="custom" totalsRowDxfId="5" dataCellStyle="Currency">
       <calculatedColumnFormula>Table7[[#This Row],[Cost (Ea)]]*Table7[[#This Row],[Qty]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(I2:I7)</totalsRowFormula>
     </tableColumn>
@@ -1608,7 +1625,7 @@
     <tableColumn id="6" name="Description"/>
     <tableColumn id="7" name="OrderNo (Rapid/Mouser)"/>
     <tableColumn id="8" name="Cost (Ea)" totalsRowLabel="Total"/>
-    <tableColumn id="9" name="Cost" totalsRowFunction="custom" totalsRowDxfId="5" dataCellStyle="Currency">
+    <tableColumn id="9" name="Cost" totalsRowFunction="custom" totalsRowDxfId="4" dataCellStyle="Currency">
       <calculatedColumnFormula>Table6[[#This Row],[Cost (Ea)]]*Table6[[#This Row],[Qty]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(I2:I21)</totalsRowFormula>
     </tableColumn>
@@ -1632,7 +1649,7 @@
     <tableColumn id="6" name="Description"/>
     <tableColumn id="7" name="OrderNo (Rapid/Mouser)"/>
     <tableColumn id="8" name="Cost (Ea)" totalsRowLabel="Total"/>
-    <tableColumn id="9" name="Cost" totalsRowFunction="custom" totalsRowDxfId="0" dataCellStyle="Currency">
+    <tableColumn id="9" name="Cost" totalsRowFunction="custom" totalsRowDxfId="3" dataCellStyle="Currency">
       <calculatedColumnFormula>Table5[[#This Row],[Cost (Ea)]]*Table5[[#This Row],[Qty]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(I2:I26)</totalsRowFormula>
     </tableColumn>
@@ -1643,7 +1660,7 @@
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:I19" totalsRowCount="1">
-  <autoFilter ref="A1:I19"/>
+  <autoFilter ref="A1:I18"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Qty"/>
     <tableColumn id="2" name="Value"/>
@@ -1653,7 +1670,7 @@
     <tableColumn id="6" name="Description"/>
     <tableColumn id="7" name="OrderNo (Rapid/Mouser)"/>
     <tableColumn id="8" name="Cost (Ea)" totalsRowLabel="Total"/>
-    <tableColumn id="9" name="Cost" totalsRowFunction="custom" totalsRowDxfId="3" dataCellStyle="Currency">
+    <tableColumn id="9" name="Cost" totalsRowFunction="custom" totalsRowDxfId="2" dataCellStyle="Currency">
       <calculatedColumnFormula>Table4[[#This Row],[Cost (Ea)]]*Table4[[#This Row],[Qty]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(I2:I18)</totalsRowFormula>
     </tableColumn>
@@ -1664,7 +1681,7 @@
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:I14" totalsRowCount="1">
-  <autoFilter ref="A1:I14"/>
+  <autoFilter ref="A1:I13"/>
   <tableColumns count="9">
     <tableColumn id="1" name="Qty"/>
     <tableColumn id="2" name="Value"/>
@@ -1674,7 +1691,7 @@
     <tableColumn id="6" name="Description"/>
     <tableColumn id="7" name="OrderNo (Rapid/Mouser)"/>
     <tableColumn id="8" name="Cost (Ea)" totalsRowLabel="Total"/>
-    <tableColumn id="9" name="Cost" totalsRowFunction="custom" totalsRowDxfId="4" dataCellStyle="Currency">
+    <tableColumn id="9" name="Cost" totalsRowFunction="custom" totalsRowDxfId="1" dataCellStyle="Currency">
       <calculatedColumnFormula>Table3[[#This Row],[Cost (Ea)]]*Table3[[#This Row],[Qty]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(I2:I13)</totalsRowFormula>
     </tableColumn>
@@ -1685,7 +1702,7 @@
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A2:B10" totalsRowCount="1">
-  <autoFilter ref="A2:B10"/>
+  <autoFilter ref="A2:B9"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Device" totalsRowLabel="Total Cost"/>
     <tableColumn id="2" name="Cost" totalsRowFunction="custom" dataCellStyle="Currency">
@@ -1697,12 +1714,12 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="A13:B16" totalsRowCount="1">
-  <autoFilter ref="A13:B16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="D2:E5" totalsRowCount="1">
+  <autoFilter ref="D2:E4"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Item" totalsRowLabel="Total Cost"/>
     <tableColumn id="2" name="Cost" totalsRowFunction="custom" dataCellStyle="Currency">
-      <totalsRowFormula>SUM(B14:B15)</totalsRowFormula>
+      <totalsRowFormula>SUM(E3:E4)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1975,7 +1992,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="B1" sqref="B1:I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2656,14 +2673,15 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H2"/>
+      <selection activeCell="I5" sqref="A1:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2807,7 +2825,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection sqref="A1:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3045,7 +3063,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection sqref="A1:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3696,7 +3714,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="I27" sqref="A1:I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4505,8 +4523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5072,7 +5090,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:H4"/>
+      <selection sqref="A1:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5482,64 +5500,132 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" t="s">
+        <v>228</v>
+      </c>
+      <c r="G2" t="s">
+        <v>263</v>
+      </c>
+      <c r="H2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>114</v>
       </c>
       <c r="B3" s="3">
         <v>11.54</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E3" s="3">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H3" s="3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>252</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="3">
+        <v>40.54</v>
+      </c>
+      <c r="G4" t="s">
+        <v>260</v>
+      </c>
+      <c r="H4" s="3">
+        <f>-(Table8[[#Totals],[Cost]])</f>
+        <v>-49.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>253</v>
       </c>
       <c r="B5" s="3">
         <v>1.1399999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>256</v>
+      </c>
+      <c r="E5" s="3">
+        <f>SUM(E3:E4)</f>
+        <v>50.54</v>
+      </c>
+      <c r="G5" t="s">
+        <v>258</v>
+      </c>
+      <c r="H5" s="3">
+        <f>-(Table10[[#Totals],[Cost]])</f>
+        <v>-50.54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>116</v>
       </c>
       <c r="B6" s="3">
         <v>12.04</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>264</v>
+      </c>
+      <c r="H6" s="3">
+        <f>SUM(H3:H5)</f>
+        <v>39.869999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>254</v>
       </c>
@@ -5547,7 +5633,7 @@
         <v>9.2100000000000009</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>118</v>
       </c>
@@ -5555,7 +5641,7 @@
         <v>8.0299999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>255</v>
       </c>
@@ -5563,99 +5649,13 @@
         <v>6.63</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>256</v>
       </c>
       <c r="B10" s="3">
         <f>SUM(B3:B9)</f>
         <v>49.59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>263</v>
-      </c>
-      <c r="B13" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>261</v>
-      </c>
-      <c r="B14" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>262</v>
-      </c>
-      <c r="B15" s="3">
-        <v>40.54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>256</v>
-      </c>
-      <c r="B16" s="3">
-        <f>SUM(B14:B15)</f>
-        <v>50.54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>263</v>
-      </c>
-      <c r="B20" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>259</v>
-      </c>
-      <c r="B21" s="3">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>260</v>
-      </c>
-      <c r="B22" s="3">
-        <f>-(Table8[[#Totals],[Cost]])</f>
-        <v>-49.59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>258</v>
-      </c>
-      <c r="B23" s="3">
-        <f>-(Table10[[#Totals],[Cost]])</f>
-        <v>-50.54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>265</v>
-      </c>
-      <c r="B24" s="3">
-        <f>SUM(B21:B23)</f>
-        <v>39.869999999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>